<commit_message>
Finalized scs 1989 builds, developing 1990
</commit_message>
<xml_diff>
--- a/inst/extdata/scs.1990/1990_Tow.xlsx
+++ b/inst/extdata/scs.1990/1990_Tow.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LarocqueY\Documents\1990\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SuretteTJ\Desktop\gulf.manage\inst\extdata\scs.1990\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -864,15 +864,6 @@
     <t>255</t>
   </si>
   <si>
-    <t>Le chalut c'est mêlé, lr fond est de la roche</t>
-  </si>
-  <si>
-    <t>terrain rought, les sensor indique des valeurs bizarre(height sensor)</t>
-  </si>
-  <si>
-    <t>Terrain rought, difficulté avec les sensors.  Enlever le sensor de temperature pour voir si il n'y a pas d'interference.</t>
-  </si>
-  <si>
     <t>Le height sensor ne fonctionne pas bien.</t>
   </si>
   <si>
@@ -882,24 +873,9 @@
     <t>Le chalut n'a pas bien chaluté(mêlé)</t>
   </si>
   <si>
-    <t>Bon trait de chalut, une grosse poche.</t>
-  </si>
-  <si>
     <t>quelques petites roches</t>
   </si>
   <si>
-    <t>terrain rought, 3 petites roches(100 lbs)</t>
-  </si>
-  <si>
-    <t>Le chalut n'a pas touché le fond, il naviguait entre deux eaux.</t>
-  </si>
-  <si>
-    <t>Une grosse roche, quelquespetites roches</t>
-  </si>
-  <si>
-    <t>Le chalut a bien fonctionné, une grosse poche</t>
-  </si>
-  <si>
     <t>Terrain vaseux</t>
   </si>
   <si>
@@ -915,138 +891,45 @@
     <t>Le height sensor est déchargé.  On va faire un autre tow avant d'aller au quai.</t>
   </si>
   <si>
-    <t>Le plotter system a perdu toute configuration ou contact avec le cabinet, donc nous n'avons pas de graphe sur l'imprimante</t>
-  </si>
-  <si>
     <t>on vient de casser un transfert</t>
   </si>
   <si>
-    <t>Je crois d'après le scanmar, le chalut n'a chaluté que 30 sec a 1 minute.</t>
-  </si>
-  <si>
-    <t>Le graphe du scanmar indique que le chalut n'a pas touché le fond avant 15h47 i.e 4 minutes avant qu'elle puisse le touché, la raison que l'on suppose est qu'il ait un courant très fort.  Le chalut a dragué pour les 5 minutes réglementaires.  Grosse roches avec trou.</t>
-  </si>
-  <si>
-    <t>Le tow # 8 a été positionné dans un autre quadrilatère 4 miles plus loin que le point original du tow 7, alors on a dû recommencer le tow.  Courant très fort, difficile a garder le chalut au fond.</t>
-  </si>
-  <si>
-    <t>Terrain rought, plusieurs petites roches, un très grosse roche</t>
-  </si>
-  <si>
-    <t>Terrain rought, 2 petites roche(25-30lbs)</t>
-  </si>
-  <si>
-    <t>Terrain rought, on a dû monter le chalut avant le temps réglementaire de 5 minutes.  Bon trait de chalut, on a dragué 4 minutes a cause du terrain rought.  2 roche (50 lbs)</t>
-  </si>
-  <si>
-    <t>Terrain un peu rought, 2 gros cailloux</t>
-  </si>
-  <si>
     <t>Terrain rought</t>
   </si>
   <si>
     <t>Terrain un peu rought.</t>
   </si>
   <si>
-    <t>Nous avons accroché une ligne de trappe carré(ligne de 50 trappes), nous en avons monté une dont 72 crabes a majorité blancs, nous avons coupé le web de la trappe, noter la position, placer une balloune et envoyer l'information au MPO. 2 trappes carré dans le chalut.  Le chalut est brisé pas mal</t>
-  </si>
-  <si>
-    <t>Terrain rought, le chalut est pas mal déchirer, les gars vont l'arranger, rien dans la poche, il faut reprendre le trait a une autre position.</t>
-  </si>
-  <si>
-    <t>Terrain rought, la poche est déchirer, 3 groses pierres de tombe dans le chalut. Il faut reprendre le tow.</t>
-  </si>
-  <si>
-    <t>Nous avons du monter le chalut avant les 5 minutes réglementaires car les portes ont accroché sur quelque chose.  Temps de chalutage, 4min 25 sec.  Le chalut est completement brisé, il faut reprendre le tow.</t>
-  </si>
-  <si>
-    <t>Seulement dragué 2 minutes, le chalut a accroché quelque choses(roches)</t>
-  </si>
-  <si>
-    <t>Seulement dragué 2 minutes car nous avons accroché deux énormes cailloux, chalut déchirer.</t>
-  </si>
-  <si>
     <t>ligne de trappe avec poche de bouette accroché en montant le chalut.</t>
   </si>
   <si>
-    <t>Le chalut est un peu déchirer, 3 gros cailloux</t>
-  </si>
-  <si>
-    <t>4 grosses roches dans la poche, le chalut est un peu brisé</t>
-  </si>
-  <si>
-    <t>3 gros cailloux dans la poche, le chalut est un peu brisé mais le trait est bon</t>
-  </si>
-  <si>
-    <t>3 énormes cailloux dans la poche.  Impossible de le monter a bord, on la soulever a coté du bateau.  Le chalut est en miette.</t>
-  </si>
-  <si>
-    <t>Seulement dragué deux minutes, le chalut a accroché quelque chose.  5 a 6 roches dans la poche.</t>
-  </si>
-  <si>
     <t>Le height sensor n'indique pas les données espérés.</t>
   </si>
   <si>
-    <t>le chalut a accroché une grosse roche platte ou une trappe, le chalut est déchirer.</t>
-  </si>
-  <si>
-    <t>roche dans la poche, poche déchirée</t>
-  </si>
-  <si>
-    <t>4 grosses pieres de tombe, le chalut est completement brisé.</t>
-  </si>
-  <si>
-    <t>Chalut completement endommagé, il faut le changé.</t>
-  </si>
-  <si>
-    <t>fond très rocheux, il faut levé apres 4 minutes.  3 roche 60 cm</t>
-  </si>
-  <si>
-    <t>Une porte a accroché après 3 minutes, il faut remonter le chalut</t>
-  </si>
-  <si>
     <t>10 cailloux 20 cm diametre</t>
   </si>
   <si>
     <t>30 cailloux 20 cm</t>
   </si>
   <si>
-    <t>fond très vaseux avec ophiures, grosse poche</t>
-  </si>
-  <si>
-    <t>Fond très rought, le chalut est très endommagé</t>
-  </si>
-  <si>
     <t>2 roches 20 cm</t>
   </si>
   <si>
     <t>fond dur</t>
   </si>
   <si>
-    <t>Fond très dur, 3 roches 40 cm</t>
-  </si>
-  <si>
     <t>2 cailloux 80 cm pris a la fin du trait</t>
   </si>
   <si>
     <t>2 tonnes de cailloux c a d 50 roches entre 30 et 50 cm de diametre</t>
   </si>
   <si>
-    <t>Chalut remonté apres 2 min, fond très rought, 1 gros cailloux</t>
-  </si>
-  <si>
     <t>100 roches 5-15 cm et un gros cailloux 1000  lbs accroché a la fin du trait</t>
   </si>
   <si>
     <t>fond très vaseux(molle)</t>
   </si>
   <si>
-    <t>10 petits cailloux 20 cm, 1 cailloux 40 cm et 1 de 80 cm</t>
-  </si>
-  <si>
-    <t>2 gros cailloux, la poche est toute defaite, il faut reprendre le trait</t>
-  </si>
-  <si>
     <t>1 gros cailloux</t>
   </si>
   <si>
@@ -1056,18 +939,12 @@
     <t>ce carré ne sera pas chaluté cette année puisque l'an passé nous avons essayé a 2deux reprise et ca n'a pas fonctionné aussi.</t>
   </si>
   <si>
-    <t>fond très vaseux avec ophiures, grosse poche.</t>
-  </si>
-  <si>
     <t>Fond très vaseux avec ophiures</t>
   </si>
   <si>
     <t>fond de gravier melanger avec vase</t>
   </si>
   <si>
-    <t>Fond très vaseux, vase molle avec ophiures</t>
-  </si>
-  <si>
     <t>Vase très molle avec ophiures</t>
   </si>
   <si>
@@ -1077,18 +954,12 @@
     <t>courant tres fort</t>
   </si>
   <si>
-    <t>Le chalut c'est enroché apres 4 min, on l'a remonté</t>
-  </si>
-  <si>
     <t>Batterie du thermometre fini</t>
   </si>
   <si>
     <t>1 caillou 30 cm de diamètre</t>
   </si>
   <si>
-    <t>Gros cailloux, la poche du chalut a été ouvert a coté du bateau.  Chalut toute déchiré.</t>
-  </si>
-  <si>
     <t>Accroché avant la fin du trait.  Trait bon</t>
   </si>
   <si>
@@ -1107,21 +978,12 @@
     <t>plusieurs gros cailloux(50 cm diametre)</t>
   </si>
   <si>
-    <t>Chalut brisé, grosse roches plate.  Perdu la peau de la poche.</t>
-  </si>
-  <si>
     <t>beaucoup de petit cailloux</t>
   </si>
   <si>
     <t>Changer la position de chalutage d'environ ¼ de mile pour éviter un autre bateau qui fait du chalutage a la position indiquer sur la carte.  On a arrêté de chaluter avant parcque ca accrochait.</t>
   </si>
   <si>
-    <t>2 gros cailloux, le coup est bon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">un caillou de 40 a 50 cm de diamètre, chalut brisé d'un bout à l'autre </t>
-  </si>
-  <si>
     <t>accroché avant la fin du coup de chalut a 3 min 30 sec.  Calut brisé</t>
   </si>
   <si>
@@ -1131,15 +993,9 @@
     <t>Chalut déchiré.  Il y avait un gros cailloux de 1 mètre de diamètre qui a été jeté a l'exterieur de la lisse.</t>
   </si>
   <si>
-    <t>10 gros cailloux, coup est bon, chalut pas brisé.</t>
-  </si>
-  <si>
     <t>Chalut déchiré au complet.  On doit reprendre le coup de chalut.</t>
   </si>
   <si>
-    <t>Chalut brisé, le coup doit être repris.</t>
-  </si>
-  <si>
     <t>Chalut brisé a nouveau.  Plusieurs gros cailloux (50-80 cm)</t>
   </si>
   <si>
@@ -1158,9 +1014,6 @@
     <t>Accroché avant la fin du 5 min.  Chaluter pendant 3 min.</t>
   </si>
   <si>
-    <t>3 gros cailloux, un aile du chalut est toute brisé.</t>
-  </si>
-  <si>
     <t>20 cailloux 15 cm</t>
   </si>
   <si>
@@ -1182,9 +1035,6 @@
     <t>On pense que le chalut n'a pas dragué sur le fond pour les 5 minutes réglementaire.  On va recommencer le trait en donnant plus de câble.</t>
   </si>
   <si>
-    <t>La poche est rempli de roche, il faut la déchirée car c'est impossible de la monter a bord.</t>
-  </si>
-  <si>
     <t>beaucoup de petite roche.</t>
   </si>
   <si>
@@ -1194,19 +1044,169 @@
     <t>Trop de courant pour la température</t>
   </si>
   <si>
-    <t>Le trait n'est pas bon, la poche est déchirée(roches)</t>
-  </si>
-  <si>
     <t>Comparaison avec Opilio</t>
   </si>
   <si>
-    <t>Comparaison avec Opilio, Vaseux</t>
-  </si>
-  <si>
-    <t>Comparaison avec Opilio, vaseux</t>
-  </si>
-  <si>
-    <t>Comparaison avec Opilio, moins vaseux</t>
+    <t>Le chalut c'est mêlé; lr fond est de la roche</t>
+  </si>
+  <si>
+    <t>terrain rought; les sensor indique des valeurs bizarre(height sensor)</t>
+  </si>
+  <si>
+    <t>Terrain rought; difficulté avec les sensors.  Enlever le sensor de temperature pour voir si il n'y a pas d'interference.</t>
+  </si>
+  <si>
+    <t>Bon trait de chalut; une grosse poche.</t>
+  </si>
+  <si>
+    <t>terrain rought; 3 petites roches(100 lbs)</t>
+  </si>
+  <si>
+    <t>Le chalut n'a pas touché le fond; il naviguait entre deux eaux.</t>
+  </si>
+  <si>
+    <t>Une grosse roche; quelquespetites roches</t>
+  </si>
+  <si>
+    <t>Le chalut a bien fonctionné; une grosse poche</t>
+  </si>
+  <si>
+    <t>Le plotter system a perdu toute configuration ou contact avec le cabinet; donc nous n'avons pas de graphe sur l'imprimante</t>
+  </si>
+  <si>
+    <t>Je crois d'après le scanmar; le chalut n'a chaluté que 30 sec a 1 minute.</t>
+  </si>
+  <si>
+    <t>Le graphe du scanmar indique que le chalut n'a pas touché le fond avant 15h47 i.e 4 minutes avant qu'elle puisse le touché; la raison que l'on suppose est qu'il ait un courant très fort.  Le chalut a dragué pour les 5 minutes réglementaires.  Grosse roches avec trou.</t>
+  </si>
+  <si>
+    <t>Le tow # 8 a été positionné dans un autre quadrilatère 4 miles plus loin que le point original du tow 7; alors on a dû recommencer le tow.  Courant très fort; difficile a garder le chalut au fond.</t>
+  </si>
+  <si>
+    <t>Terrain rought; plusieurs petites roches; un très grosse roche</t>
+  </si>
+  <si>
+    <t>Terrain rought; 2 petites roche(25-30lbs)</t>
+  </si>
+  <si>
+    <t>Terrain rought; on a dû monter le chalut avant le temps réglementaire de 5 minutes.  Bon trait de chalut; on a dragué 4 minutes a cause du terrain rought.  2 roche (50 lbs)</t>
+  </si>
+  <si>
+    <t>Terrain un peu rought; 2 gros cailloux</t>
+  </si>
+  <si>
+    <t>Nous avons accroché une ligne de trappe carré(ligne de 50 trappes); nous en avons monté une dont 72 crabes a majorité blancs; nous avons coupé le web de la trappe; noter la position; placer une balloune et envoyer l'information au MPO. 2 trappes carré dans le chalut.  Le chalut est brisé pas mal</t>
+  </si>
+  <si>
+    <t>Terrain rought; le chalut est pas mal déchirer; les gars vont l'arranger; rien dans la poche; il faut reprendre le trait a une autre position.</t>
+  </si>
+  <si>
+    <t>Terrain rought; la poche est déchirer; 3 groses pierres de tombe dans le chalut. Il faut reprendre le tow.</t>
+  </si>
+  <si>
+    <t>Nous avons du monter le chalut avant les 5 minutes réglementaires car les portes ont accroché sur quelque chose.  Temps de chalutage; 4min 25 sec.  Le chalut est completement brisé; il faut reprendre le tow.</t>
+  </si>
+  <si>
+    <t>Seulement dragué 2 minutes; le chalut a accroché quelque choses(roches)</t>
+  </si>
+  <si>
+    <t>Seulement dragué 2 minutes car nous avons accroché deux énormes cailloux; chalut déchirer.</t>
+  </si>
+  <si>
+    <t>Le chalut est un peu déchirer; 3 gros cailloux</t>
+  </si>
+  <si>
+    <t>4 grosses roches dans la poche; le chalut est un peu brisé</t>
+  </si>
+  <si>
+    <t>3 gros cailloux dans la poche; le chalut est un peu brisé mais le trait est bon</t>
+  </si>
+  <si>
+    <t>3 énormes cailloux dans la poche.  Impossible de le monter a bord; on la soulever a coté du bateau.  Le chalut est en miette.</t>
+  </si>
+  <si>
+    <t>Seulement dragué deux minutes; le chalut a accroché quelque chose.  5 a 6 roches dans la poche.</t>
+  </si>
+  <si>
+    <t>le chalut a accroché une grosse roche platte ou une trappe; le chalut est déchirer.</t>
+  </si>
+  <si>
+    <t>roche dans la poche; poche déchirée</t>
+  </si>
+  <si>
+    <t>4 grosses pieres de tombe; le chalut est completement brisé.</t>
+  </si>
+  <si>
+    <t>Chalut completement endommagé; il faut le changé.</t>
+  </si>
+  <si>
+    <t>fond très rocheux; il faut levé apres 4 minutes.  3 roche 60 cm</t>
+  </si>
+  <si>
+    <t>Une porte a accroché après 3 minutes; il faut remonter le chalut</t>
+  </si>
+  <si>
+    <t>fond très vaseux avec ophiures; grosse poche</t>
+  </si>
+  <si>
+    <t>Fond très rought; le chalut est très endommagé</t>
+  </si>
+  <si>
+    <t>Fond très dur; 3 roches 40 cm</t>
+  </si>
+  <si>
+    <t>Chalut remonté apres 2 min; fond très rought; 1 gros cailloux</t>
+  </si>
+  <si>
+    <t>10 petits cailloux 20 cm; 1 cailloux 40 cm et 1 de 80 cm</t>
+  </si>
+  <si>
+    <t>2 gros cailloux; la poche est toute defaite; il faut reprendre le trait</t>
+  </si>
+  <si>
+    <t>fond très vaseux avec ophiures; grosse poche.</t>
+  </si>
+  <si>
+    <t>Fond très vaseux; vase molle avec ophiures</t>
+  </si>
+  <si>
+    <t>Le chalut c'est enroché apres 4 min; on l'a remonté</t>
+  </si>
+  <si>
+    <t>Gros cailloux; la poche du chalut a été ouvert a coté du bateau.  Chalut toute déchiré.</t>
+  </si>
+  <si>
+    <t>Chalut brisé; grosse roches plate.  Perdu la peau de la poche.</t>
+  </si>
+  <si>
+    <t>2 gros cailloux; le coup est bon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">un caillou de 40 a 50 cm de diamètre; chalut brisé d'un bout à l'autre </t>
+  </si>
+  <si>
+    <t>10 gros cailloux; coup est bon; chalut pas brisé.</t>
+  </si>
+  <si>
+    <t>Chalut brisé; le coup doit être repris.</t>
+  </si>
+  <si>
+    <t>3 gros cailloux; un aile du chalut est toute brisé.</t>
+  </si>
+  <si>
+    <t>La poche est rempli de roche; il faut la déchirée car c'est impossible de la monter a bord.</t>
+  </si>
+  <si>
+    <t>Le trait n'est pas bon; la poche est déchirée(roches)</t>
+  </si>
+  <si>
+    <t>Comparaison avec Opilio; Vaseux</t>
+  </si>
+  <si>
+    <t>Comparaison avec Opilio; vaseux</t>
+  </si>
+  <si>
+    <t>Comparaison avec Opilio; moins vaseux</t>
   </si>
 </sst>
 </file>
@@ -1729,48 +1729,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1786,7 +1786,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2051,31 +2051,31 @@
   <dimension ref="A1:U296"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A276" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="S293" sqref="S293"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
-    <col min="6" max="6" width="6.81640625" customWidth="1"/>
-    <col min="7" max="7" width="7.1796875" customWidth="1"/>
-    <col min="8" max="8" width="6.36328125" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
+    <col min="6" max="6" width="6.85546875" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" customWidth="1"/>
     <col min="9" max="9" width="7" customWidth="1"/>
-    <col min="10" max="10" width="8.7265625" style="2"/>
-    <col min="11" max="11" width="7.08984375" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="2"/>
-    <col min="13" max="13" width="8.7265625" style="4"/>
-    <col min="14" max="14" width="7.36328125" customWidth="1"/>
-    <col min="15" max="15" width="8.08984375" customWidth="1"/>
-    <col min="16" max="16" width="6.7265625" customWidth="1"/>
-    <col min="17" max="17" width="8.08984375" customWidth="1"/>
-    <col min="18" max="18" width="6.90625" customWidth="1"/>
-    <col min="19" max="19" width="23.36328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" style="2"/>
+    <col min="11" max="11" width="7.140625" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="2"/>
+    <col min="13" max="13" width="8.7109375" style="4"/>
+    <col min="14" max="14" width="7.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" customWidth="1"/>
+    <col min="16" max="16" width="6.7109375" customWidth="1"/>
+    <col min="17" max="17" width="8.140625" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" customWidth="1"/>
+    <col min="19" max="19" width="23.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2140,7 +2140,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1990</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>22</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>281</v>
+        <v>342</v>
       </c>
       <c r="T2" t="s">
         <v>23</v>
@@ -2202,7 +2202,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1990</v>
       </c>
@@ -2261,7 +2261,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1990</v>
       </c>
@@ -2320,7 +2320,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1990</v>
       </c>
@@ -2379,7 +2379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1990</v>
       </c>
@@ -2432,7 +2432,7 @@
         <v>22</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>282</v>
+        <v>343</v>
       </c>
       <c r="T6" t="s">
         <v>23</v>
@@ -2441,7 +2441,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1990</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>22</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>283</v>
+        <v>344</v>
       </c>
       <c r="T7" t="s">
         <v>23</v>
@@ -2503,7 +2503,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1990</v>
       </c>
@@ -2562,7 +2562,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1990</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>22</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="T9" t="s">
         <v>23</v>
@@ -2624,7 +2624,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1990</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1990</v>
       </c>
@@ -2742,7 +2742,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1990</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1990</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1990</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1990</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1990</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>22</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="T16" t="s">
         <v>23</v>
@@ -3040,7 +3040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1990</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1990</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1990</v>
       </c>
@@ -3214,7 +3214,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1990</v>
       </c>
@@ -3267,7 +3267,7 @@
         <v>22</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="T20" t="s">
         <v>23</v>
@@ -3276,7 +3276,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1990</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>22</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="T21" t="s">
         <v>23</v>
@@ -3338,7 +3338,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1990</v>
       </c>
@@ -3391,7 +3391,7 @@
         <v>22</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="T22" t="s">
         <v>23</v>
@@ -3400,7 +3400,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1990</v>
       </c>
@@ -3453,7 +3453,7 @@
         <v>22</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="T23" t="s">
         <v>23</v>
@@ -3462,7 +3462,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1990</v>
       </c>
@@ -3515,7 +3515,7 @@
         <v>22</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>289</v>
+        <v>346</v>
       </c>
       <c r="T24" t="s">
         <v>23</v>
@@ -3524,7 +3524,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1990</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1990</v>
       </c>
@@ -3642,7 +3642,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1990</v>
       </c>
@@ -3701,7 +3701,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>1990</v>
       </c>
@@ -3760,7 +3760,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1990</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1990</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>22</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>287</v>
+        <v>345</v>
       </c>
       <c r="T30" t="s">
         <v>23</v>
@@ -3881,7 +3881,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1990</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1990</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>1990</v>
       </c>
@@ -4058,7 +4058,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1990</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>22</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>290</v>
+        <v>347</v>
       </c>
       <c r="T34" t="s">
         <v>23</v>
@@ -4120,7 +4120,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>1990</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>22</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>291</v>
+        <v>348</v>
       </c>
       <c r="T35" t="s">
         <v>23</v>
@@ -4182,7 +4182,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1990</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>22</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>292</v>
+        <v>349</v>
       </c>
       <c r="T36" t="s">
         <v>23</v>
@@ -4244,7 +4244,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1990</v>
       </c>
@@ -4303,7 +4303,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>1990</v>
       </c>
@@ -4356,7 +4356,7 @@
         <v>22</v>
       </c>
       <c r="S38" s="1" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="T38" t="s">
         <v>23</v>
@@ -4365,7 +4365,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>1990</v>
       </c>
@@ -4418,7 +4418,7 @@
         <v>22</v>
       </c>
       <c r="S39" s="1" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="T39" t="s">
         <v>23</v>
@@ -4427,7 +4427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>1990</v>
       </c>
@@ -4480,7 +4480,7 @@
         <v>22</v>
       </c>
       <c r="S40" s="1" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="T40" t="s">
         <v>23</v>
@@ -4489,7 +4489,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1990</v>
       </c>
@@ -4542,7 +4542,7 @@
         <v>22</v>
       </c>
       <c r="S41" s="1" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="T41" t="s">
         <v>23</v>
@@ -4551,7 +4551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>1990</v>
       </c>
@@ -4604,7 +4604,7 @@
         <v>22</v>
       </c>
       <c r="S42" s="1" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="T42" t="s">
         <v>23</v>
@@ -4613,7 +4613,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>1990</v>
       </c>
@@ -4672,7 +4672,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1990</v>
       </c>
@@ -4731,7 +4731,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>1990</v>
       </c>
@@ -4784,7 +4784,7 @@
         <v>22</v>
       </c>
       <c r="S45" s="1" t="s">
-        <v>298</v>
+        <v>350</v>
       </c>
       <c r="T45" t="s">
         <v>23</v>
@@ -4793,7 +4793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>1990</v>
       </c>
@@ -4852,7 +4852,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>1990</v>
       </c>
@@ -4905,7 +4905,7 @@
         <v>22</v>
       </c>
       <c r="S47" s="1" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="T47" t="s">
         <v>23</v>
@@ -4914,7 +4914,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>1990</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>1990</v>
       </c>
@@ -5032,7 +5032,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>1990</v>
       </c>
@@ -5091,7 +5091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>1990</v>
       </c>
@@ -5144,7 +5144,7 @@
         <v>22</v>
       </c>
       <c r="S51" s="1" t="s">
-        <v>300</v>
+        <v>351</v>
       </c>
       <c r="T51" t="s">
         <v>23</v>
@@ -5153,7 +5153,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>1990</v>
       </c>
@@ -5206,7 +5206,7 @@
         <v>22</v>
       </c>
       <c r="S52" s="1" t="s">
-        <v>301</v>
+        <v>352</v>
       </c>
       <c r="T52" t="s">
         <v>23</v>
@@ -5215,7 +5215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>1990</v>
       </c>
@@ -5268,7 +5268,7 @@
         <v>22</v>
       </c>
       <c r="S53" s="1" t="s">
-        <v>302</v>
+        <v>353</v>
       </c>
       <c r="T53" t="s">
         <v>23</v>
@@ -5277,7 +5277,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>1990</v>
       </c>
@@ -5336,7 +5336,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>1990</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>1990</v>
       </c>
@@ -5448,7 +5448,7 @@
         <v>22</v>
       </c>
       <c r="S56" s="1" t="s">
-        <v>303</v>
+        <v>354</v>
       </c>
       <c r="T56" t="s">
         <v>23</v>
@@ -5457,7 +5457,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>1990</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>22</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>304</v>
+        <v>355</v>
       </c>
       <c r="T57" t="s">
         <v>23</v>
@@ -5519,7 +5519,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>1990</v>
       </c>
@@ -5572,7 +5572,7 @@
         <v>22</v>
       </c>
       <c r="S58" s="1" t="s">
-        <v>305</v>
+        <v>356</v>
       </c>
       <c r="T58" t="s">
         <v>23</v>
@@ -5581,7 +5581,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1990</v>
       </c>
@@ -5634,7 +5634,7 @@
         <v>22</v>
       </c>
       <c r="S59" s="1" t="s">
-        <v>306</v>
+        <v>357</v>
       </c>
       <c r="T59" t="s">
         <v>23</v>
@@ -5643,7 +5643,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>1990</v>
       </c>
@@ -5696,7 +5696,7 @@
         <v>22</v>
       </c>
       <c r="S60" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="T60" t="s">
         <v>23</v>
@@ -5705,7 +5705,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>1990</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>22</v>
       </c>
       <c r="S61" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="T61" t="s">
         <v>23</v>
@@ -5767,7 +5767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1990</v>
       </c>
@@ -5826,7 +5826,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>1990</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>1990</v>
       </c>
@@ -5938,7 +5938,7 @@
         <v>22</v>
       </c>
       <c r="S64" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="T64" t="s">
         <v>23</v>
@@ -5947,7 +5947,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>1990</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>22</v>
       </c>
       <c r="S65" s="1" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="T65" t="s">
         <v>23</v>
@@ -6009,7 +6009,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>1990</v>
       </c>
@@ -6068,7 +6068,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>1990</v>
       </c>
@@ -6127,7 +6127,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>1990</v>
       </c>
@@ -6186,7 +6186,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
         <v>1990</v>
       </c>
@@ -6239,7 +6239,7 @@
         <v>22</v>
       </c>
       <c r="S69" s="5" t="s">
-        <v>309</v>
+        <v>358</v>
       </c>
       <c r="T69" s="5" t="s">
         <v>23</v>
@@ -6248,7 +6248,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>1990</v>
       </c>
@@ -6307,7 +6307,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>1990</v>
       </c>
@@ -6366,7 +6366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>1990</v>
       </c>
@@ -6419,7 +6419,7 @@
         <v>22</v>
       </c>
       <c r="S72" s="1" t="s">
-        <v>310</v>
+        <v>359</v>
       </c>
       <c r="T72" t="s">
         <v>23</v>
@@ -6428,7 +6428,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>1990</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>1990</v>
       </c>
@@ -6546,7 +6546,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>1990</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1990</v>
       </c>
@@ -6658,7 +6658,7 @@
         <v>22</v>
       </c>
       <c r="S76" s="1" t="s">
-        <v>311</v>
+        <v>360</v>
       </c>
       <c r="T76" t="s">
         <v>23</v>
@@ -6667,7 +6667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>1990</v>
       </c>
@@ -6720,7 +6720,7 @@
         <v>22</v>
       </c>
       <c r="S77" s="1" t="s">
-        <v>312</v>
+        <v>361</v>
       </c>
       <c r="T77" t="s">
         <v>23</v>
@@ -6729,7 +6729,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>1990</v>
       </c>
@@ -6782,7 +6782,7 @@
         <v>22</v>
       </c>
       <c r="S78" s="1" t="s">
-        <v>313</v>
+        <v>362</v>
       </c>
       <c r="T78" t="s">
         <v>23</v>
@@ -6791,7 +6791,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>1990</v>
       </c>
@@ -6844,7 +6844,7 @@
         <v>22</v>
       </c>
       <c r="S79" s="1" t="s">
-        <v>314</v>
+        <v>363</v>
       </c>
       <c r="T79" t="s">
         <v>23</v>
@@ -6853,7 +6853,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>1990</v>
       </c>
@@ -6906,7 +6906,7 @@
         <v>22</v>
       </c>
       <c r="S80" s="1" t="s">
-        <v>315</v>
+        <v>293</v>
       </c>
       <c r="T80" t="s">
         <v>23</v>
@@ -6915,7 +6915,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>1990</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>1990</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>1990</v>
       </c>
@@ -7092,7 +7092,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>1990</v>
       </c>
@@ -7145,7 +7145,7 @@
         <v>22</v>
       </c>
       <c r="S84" s="1" t="s">
-        <v>316</v>
+        <v>364</v>
       </c>
       <c r="T84" t="s">
         <v>23</v>
@@ -7154,7 +7154,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>1990</v>
       </c>
@@ -7213,7 +7213,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>1990</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>1990</v>
       </c>
@@ -7325,7 +7325,7 @@
         <v>22</v>
       </c>
       <c r="S87" s="1" t="s">
-        <v>317</v>
+        <v>365</v>
       </c>
       <c r="T87" t="s">
         <v>23</v>
@@ -7334,7 +7334,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>1990</v>
       </c>
@@ -7387,7 +7387,7 @@
         <v>22</v>
       </c>
       <c r="S88" s="1" t="s">
-        <v>318</v>
+        <v>366</v>
       </c>
       <c r="T88" t="s">
         <v>23</v>
@@ -7396,7 +7396,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>1990</v>
       </c>
@@ -7455,7 +7455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>1990</v>
       </c>
@@ -7508,7 +7508,7 @@
         <v>22</v>
       </c>
       <c r="S90" s="1" t="s">
-        <v>319</v>
+        <v>367</v>
       </c>
       <c r="T90" t="s">
         <v>23</v>
@@ -7517,7 +7517,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>1990</v>
       </c>
@@ -7576,7 +7576,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>1990</v>
       </c>
@@ -7629,7 +7629,7 @@
         <v>22</v>
       </c>
       <c r="S92" s="1" t="s">
-        <v>320</v>
+        <v>368</v>
       </c>
       <c r="T92" t="s">
         <v>23</v>
@@ -7638,7 +7638,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>1990</v>
       </c>
@@ -7691,7 +7691,7 @@
         <v>22</v>
       </c>
       <c r="S93" s="1" t="s">
-        <v>321</v>
+        <v>294</v>
       </c>
       <c r="T93" t="s">
         <v>23</v>
@@ -7700,7 +7700,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>1990</v>
       </c>
@@ -7759,7 +7759,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>1990</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>22</v>
       </c>
       <c r="S95" s="1" t="s">
-        <v>322</v>
+        <v>369</v>
       </c>
       <c r="T95" t="s">
         <v>23</v>
@@ -7821,7 +7821,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>1990</v>
       </c>
@@ -7874,7 +7874,7 @@
         <v>22</v>
       </c>
       <c r="S96" s="1" t="s">
-        <v>323</v>
+        <v>370</v>
       </c>
       <c r="T96" t="s">
         <v>23</v>
@@ -7883,7 +7883,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>1990</v>
       </c>
@@ -7942,7 +7942,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>1990</v>
       </c>
@@ -8001,7 +8001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>1990</v>
       </c>
@@ -8054,7 +8054,7 @@
         <v>22</v>
       </c>
       <c r="S99" s="1" t="s">
-        <v>324</v>
+        <v>371</v>
       </c>
       <c r="T99" t="s">
         <v>23</v>
@@ -8063,7 +8063,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>1990</v>
       </c>
@@ -8122,7 +8122,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>1990</v>
       </c>
@@ -8181,7 +8181,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>1990</v>
       </c>
@@ -8240,7 +8240,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>1990</v>
       </c>
@@ -8293,7 +8293,7 @@
         <v>22</v>
       </c>
       <c r="S103" s="1" t="s">
-        <v>325</v>
+        <v>372</v>
       </c>
       <c r="T103" t="s">
         <v>23</v>
@@ -8302,7 +8302,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>1990</v>
       </c>
@@ -8355,7 +8355,7 @@
         <v>22</v>
       </c>
       <c r="S104" s="1" t="s">
-        <v>326</v>
+        <v>373</v>
       </c>
       <c r="T104" t="s">
         <v>23</v>
@@ -8364,7 +8364,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>1990</v>
       </c>
@@ -8417,7 +8417,7 @@
         <v>22</v>
       </c>
       <c r="S105" s="1" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
       <c r="T105" t="s">
         <v>23</v>
@@ -8426,7 +8426,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1990</v>
       </c>
@@ -8479,7 +8479,7 @@
         <v>22</v>
       </c>
       <c r="S106" s="1" t="s">
-        <v>327</v>
+        <v>374</v>
       </c>
       <c r="T106" t="s">
         <v>23</v>
@@ -8488,7 +8488,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>1990</v>
       </c>
@@ -8547,7 +8547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>1990</v>
       </c>
@@ -8600,7 +8600,7 @@
         <v>22</v>
       </c>
       <c r="S108" s="1" t="s">
-        <v>328</v>
+        <v>295</v>
       </c>
       <c r="T108" t="s">
         <v>23</v>
@@ -8609,7 +8609,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1990</v>
       </c>
@@ -8662,7 +8662,7 @@
         <v>22</v>
       </c>
       <c r="S109" s="1" t="s">
-        <v>329</v>
+        <v>296</v>
       </c>
       <c r="T109" t="s">
         <v>23</v>
@@ -8671,7 +8671,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>1990</v>
       </c>
@@ -8730,7 +8730,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>1990</v>
       </c>
@@ -8783,7 +8783,7 @@
         <v>22</v>
       </c>
       <c r="S111" s="1" t="s">
-        <v>330</v>
+        <v>375</v>
       </c>
       <c r="T111" t="s">
         <v>23</v>
@@ -8792,7 +8792,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>1990</v>
       </c>
@@ -8845,7 +8845,7 @@
         <v>22</v>
       </c>
       <c r="S112" s="1" t="s">
-        <v>331</v>
+        <v>376</v>
       </c>
       <c r="T112" t="s">
         <v>23</v>
@@ -8854,7 +8854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1990</v>
       </c>
@@ -8907,7 +8907,7 @@
         <v>22</v>
       </c>
       <c r="S113" s="1" t="s">
-        <v>332</v>
+        <v>297</v>
       </c>
       <c r="T113" t="s">
         <v>23</v>
@@ -8916,7 +8916,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>1990</v>
       </c>
@@ -8975,7 +8975,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>1990</v>
       </c>
@@ -9034,7 +9034,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>1990</v>
       </c>
@@ -9093,7 +9093,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>1990</v>
       </c>
@@ -9146,7 +9146,7 @@
         <v>22</v>
       </c>
       <c r="S117" s="1" t="s">
-        <v>333</v>
+        <v>298</v>
       </c>
       <c r="T117" t="s">
         <v>23</v>
@@ -9155,7 +9155,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>1990</v>
       </c>
@@ -9208,7 +9208,7 @@
         <v>22</v>
       </c>
       <c r="S118" s="1" t="s">
-        <v>334</v>
+        <v>377</v>
       </c>
       <c r="T118" t="s">
         <v>23</v>
@@ -9217,7 +9217,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>1990</v>
       </c>
@@ -9270,7 +9270,7 @@
         <v>22</v>
       </c>
       <c r="S119" s="1" t="s">
-        <v>335</v>
+        <v>299</v>
       </c>
       <c r="T119" t="s">
         <v>23</v>
@@ -9279,7 +9279,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>1990</v>
       </c>
@@ -9338,7 +9338,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>1990</v>
       </c>
@@ -9397,7 +9397,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>1990</v>
       </c>
@@ -9456,7 +9456,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>1990</v>
       </c>
@@ -9509,7 +9509,7 @@
         <v>22</v>
       </c>
       <c r="S123" s="1" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
       <c r="T123" t="s">
         <v>23</v>
@@ -9518,7 +9518,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>1990</v>
       </c>
@@ -9577,7 +9577,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>1990</v>
       </c>
@@ -9636,7 +9636,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>1990</v>
       </c>
@@ -9689,7 +9689,7 @@
         <v>22</v>
       </c>
       <c r="S126" s="1" t="s">
-        <v>337</v>
+        <v>378</v>
       </c>
       <c r="T126" t="s">
         <v>23</v>
@@ -9698,7 +9698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>1990</v>
       </c>
@@ -9757,7 +9757,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>1990</v>
       </c>
@@ -9810,7 +9810,7 @@
         <v>22</v>
       </c>
       <c r="S128" s="1" t="s">
-        <v>338</v>
+        <v>301</v>
       </c>
       <c r="T128" t="s">
         <v>23</v>
@@ -9819,7 +9819,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="129" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>1990</v>
       </c>
@@ -9872,7 +9872,7 @@
         <v>22</v>
       </c>
       <c r="S129" s="1" t="s">
-        <v>339</v>
+        <v>302</v>
       </c>
       <c r="T129" t="s">
         <v>23</v>
@@ -9881,7 +9881,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>1990</v>
       </c>
@@ -9934,7 +9934,7 @@
         <v>22</v>
       </c>
       <c r="S130" s="1" t="s">
-        <v>340</v>
+        <v>379</v>
       </c>
       <c r="T130" t="s">
         <v>23</v>
@@ -9943,7 +9943,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>1990</v>
       </c>
@@ -9996,7 +9996,7 @@
         <v>22</v>
       </c>
       <c r="S131" s="1" t="s">
-        <v>341</v>
+        <v>380</v>
       </c>
       <c r="T131" t="s">
         <v>23</v>
@@ -10005,7 +10005,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="132" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>1990</v>
       </c>
@@ -10058,7 +10058,7 @@
         <v>22</v>
       </c>
       <c r="S132" s="1" t="s">
-        <v>342</v>
+        <v>303</v>
       </c>
       <c r="T132" t="s">
         <v>23</v>
@@ -10067,7 +10067,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="133" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>1990</v>
       </c>
@@ -10126,7 +10126,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>1990</v>
       </c>
@@ -10179,7 +10179,7 @@
         <v>22</v>
       </c>
       <c r="S134" s="1" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="T134" t="s">
         <v>23</v>
@@ -10188,7 +10188,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>1990</v>
       </c>
@@ -10241,7 +10241,7 @@
         <v>22</v>
       </c>
       <c r="S135" s="1" t="s">
-        <v>344</v>
+        <v>305</v>
       </c>
       <c r="T135" t="s">
         <v>23</v>
@@ -10250,7 +10250,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="136" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>1990</v>
       </c>
@@ -10309,7 +10309,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>1990</v>
       </c>
@@ -10368,7 +10368,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>1990</v>
       </c>
@@ -10427,7 +10427,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>1990</v>
       </c>
@@ -10486,7 +10486,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>1990</v>
       </c>
@@ -10545,7 +10545,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>1990</v>
       </c>
@@ -10604,7 +10604,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="142" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>1990</v>
       </c>
@@ -10663,7 +10663,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="143" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>1990</v>
       </c>
@@ -10716,7 +10716,7 @@
         <v>22</v>
       </c>
       <c r="S143" s="1" t="s">
-        <v>345</v>
+        <v>381</v>
       </c>
       <c r="T143" t="s">
         <v>23</v>
@@ -10725,7 +10725,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="144" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>1990</v>
       </c>
@@ -10778,7 +10778,7 @@
         <v>22</v>
       </c>
       <c r="S144" s="1" t="s">
-        <v>346</v>
+        <v>306</v>
       </c>
       <c r="T144" t="s">
         <v>23</v>
@@ -10787,7 +10787,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="145" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>1990</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>22</v>
       </c>
       <c r="S145" s="1" t="s">
-        <v>347</v>
+        <v>307</v>
       </c>
       <c r="T145" t="s">
         <v>23</v>
@@ -10849,7 +10849,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="146" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>1990</v>
       </c>
@@ -10908,7 +10908,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="147" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>1990</v>
       </c>
@@ -10961,7 +10961,7 @@
         <v>22</v>
       </c>
       <c r="S147" s="1" t="s">
-        <v>348</v>
+        <v>382</v>
       </c>
       <c r="T147" t="s">
         <v>23</v>
@@ -10970,7 +10970,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="148" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>1990</v>
       </c>
@@ -11023,7 +11023,7 @@
         <v>22</v>
       </c>
       <c r="S148" s="1" t="s">
-        <v>349</v>
+        <v>308</v>
       </c>
       <c r="T148" t="s">
         <v>23</v>
@@ -11032,7 +11032,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="149" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>1990</v>
       </c>
@@ -11091,7 +11091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>1990</v>
       </c>
@@ -11150,7 +11150,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="151" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>1990</v>
       </c>
@@ -11209,7 +11209,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>1990</v>
       </c>
@@ -11262,7 +11262,7 @@
         <v>22</v>
       </c>
       <c r="S152" s="1" t="s">
-        <v>342</v>
+        <v>303</v>
       </c>
       <c r="T152" t="s">
         <v>23</v>
@@ -11271,7 +11271,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>1990</v>
       </c>
@@ -11330,7 +11330,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="154" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>1990</v>
       </c>
@@ -11383,7 +11383,7 @@
         <v>22</v>
       </c>
       <c r="S154" s="1" t="s">
-        <v>343</v>
+        <v>304</v>
       </c>
       <c r="T154" t="s">
         <v>23</v>
@@ -11392,7 +11392,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>1990</v>
       </c>
@@ -11451,7 +11451,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="156" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>1990</v>
       </c>
@@ -11510,7 +11510,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>1990</v>
       </c>
@@ -11569,7 +11569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>1990</v>
       </c>
@@ -11628,7 +11628,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="159" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>1990</v>
       </c>
@@ -11687,7 +11687,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>1990</v>
       </c>
@@ -11746,7 +11746,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="161" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>1990</v>
       </c>
@@ -11805,7 +11805,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>1990</v>
       </c>
@@ -11864,7 +11864,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>1990</v>
       </c>
@@ -11923,7 +11923,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="164" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>1990</v>
       </c>
@@ -11982,7 +11982,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="165" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>1990</v>
       </c>
@@ -12041,7 +12041,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="166" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>1990</v>
       </c>
@@ -12100,7 +12100,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="167" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>1990</v>
       </c>
@@ -12159,7 +12159,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="168" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>1990</v>
       </c>
@@ -12218,7 +12218,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>1990</v>
       </c>
@@ -12277,7 +12277,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="170" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>1990</v>
       </c>
@@ -12336,7 +12336,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="171" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>1990</v>
       </c>
@@ -12395,7 +12395,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="172" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>1990</v>
       </c>
@@ -12454,7 +12454,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="173" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>1990</v>
       </c>
@@ -12513,7 +12513,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="174" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>1990</v>
       </c>
@@ -12566,7 +12566,7 @@
         <v>22</v>
       </c>
       <c r="S174" s="1" t="s">
-        <v>350</v>
+        <v>309</v>
       </c>
       <c r="T174" t="s">
         <v>23</v>
@@ -12575,7 +12575,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="175" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>1990</v>
       </c>
@@ -12634,7 +12634,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>1990</v>
       </c>
@@ -12693,7 +12693,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>1990</v>
       </c>
@@ -12752,7 +12752,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="178" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>1990</v>
       </c>
@@ -12811,7 +12811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="179" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>1990</v>
       </c>
@@ -12864,7 +12864,7 @@
         <v>22</v>
       </c>
       <c r="S179" s="1" t="s">
-        <v>351</v>
+        <v>310</v>
       </c>
       <c r="T179" t="s">
         <v>23</v>
@@ -12873,7 +12873,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="180" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>1990</v>
       </c>
@@ -12932,7 +12932,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>1990</v>
       </c>
@@ -12991,7 +12991,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="182" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>1990</v>
       </c>
@@ -13050,7 +13050,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>1990</v>
       </c>
@@ -13109,7 +13109,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="184" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>1990</v>
       </c>
@@ -13162,7 +13162,7 @@
         <v>22</v>
       </c>
       <c r="S184" s="1" t="s">
-        <v>352</v>
+        <v>383</v>
       </c>
       <c r="T184" t="s">
         <v>23</v>
@@ -13171,7 +13171,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="185" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>1990</v>
       </c>
@@ -13230,7 +13230,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="186" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>1990</v>
       </c>
@@ -13289,7 +13289,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="187" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>1990</v>
       </c>
@@ -13348,7 +13348,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="188" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>1990</v>
       </c>
@@ -13401,7 +13401,7 @@
         <v>22</v>
       </c>
       <c r="S188" s="1" t="s">
-        <v>353</v>
+        <v>311</v>
       </c>
       <c r="T188" t="s">
         <v>23</v>
@@ -13410,7 +13410,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="189" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>1990</v>
       </c>
@@ -13469,7 +13469,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="190" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>1990</v>
       </c>
@@ -13528,7 +13528,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="191" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>1990</v>
       </c>
@@ -13581,7 +13581,7 @@
         <v>22</v>
       </c>
       <c r="S191" s="1" t="s">
-        <v>354</v>
+        <v>312</v>
       </c>
       <c r="T191" t="s">
         <v>23</v>
@@ -13590,7 +13590,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="192" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>1990</v>
       </c>
@@ -13643,7 +13643,7 @@
         <v>22</v>
       </c>
       <c r="S192" s="1" t="s">
-        <v>355</v>
+        <v>384</v>
       </c>
       <c r="T192" t="s">
         <v>23</v>
@@ -13652,7 +13652,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="193" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>1990</v>
       </c>
@@ -13705,7 +13705,7 @@
         <v>22</v>
       </c>
       <c r="S193" s="1" t="s">
-        <v>356</v>
+        <v>313</v>
       </c>
       <c r="T193" t="s">
         <v>23</v>
@@ -13714,7 +13714,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="194" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>1990</v>
       </c>
@@ -13773,7 +13773,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="195" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>1990</v>
       </c>
@@ -13832,7 +13832,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="196" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>1990</v>
       </c>
@@ -13885,7 +13885,7 @@
         <v>22</v>
       </c>
       <c r="S196" s="1" t="s">
-        <v>357</v>
+        <v>314</v>
       </c>
       <c r="T196" t="s">
         <v>23</v>
@@ -13894,7 +13894,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="197" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>1990</v>
       </c>
@@ -13953,7 +13953,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="198" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>1990</v>
       </c>
@@ -14006,7 +14006,7 @@
         <v>22</v>
       </c>
       <c r="S198" s="1" t="s">
-        <v>358</v>
+        <v>315</v>
       </c>
       <c r="T198" t="s">
         <v>23</v>
@@ -14015,7 +14015,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="199" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>1990</v>
       </c>
@@ -14074,7 +14074,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="200" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>1990</v>
       </c>
@@ -14127,7 +14127,7 @@
         <v>22</v>
       </c>
       <c r="S200" s="1" t="s">
-        <v>359</v>
+        <v>316</v>
       </c>
       <c r="T200" t="s">
         <v>23</v>
@@ -14136,7 +14136,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="201" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>1990</v>
       </c>
@@ -14189,7 +14189,7 @@
         <v>22</v>
       </c>
       <c r="S201" s="1" t="s">
-        <v>360</v>
+        <v>317</v>
       </c>
       <c r="T201" t="s">
         <v>23</v>
@@ -14198,7 +14198,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="202" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>1990</v>
       </c>
@@ -14251,7 +14251,7 @@
         <v>22</v>
       </c>
       <c r="S202" s="1" t="s">
-        <v>361</v>
+        <v>318</v>
       </c>
       <c r="T202" t="s">
         <v>23</v>
@@ -14260,7 +14260,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="203" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>1990</v>
       </c>
@@ -14319,7 +14319,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="204" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>1990</v>
       </c>
@@ -14372,7 +14372,7 @@
         <v>22</v>
       </c>
       <c r="S204" s="1" t="s">
-        <v>362</v>
+        <v>385</v>
       </c>
       <c r="T204" t="s">
         <v>23</v>
@@ -14381,7 +14381,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="205" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>1990</v>
       </c>
@@ -14434,7 +14434,7 @@
         <v>22</v>
       </c>
       <c r="S205" s="1" t="s">
-        <v>363</v>
+        <v>319</v>
       </c>
       <c r="T205" t="s">
         <v>23</v>
@@ -14443,7 +14443,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="206" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>1990</v>
       </c>
@@ -14502,7 +14502,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="207" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>1990</v>
       </c>
@@ -14561,7 +14561,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="208" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>1990</v>
       </c>
@@ -14620,7 +14620,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="209" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>1990</v>
       </c>
@@ -14673,7 +14673,7 @@
         <v>22</v>
       </c>
       <c r="S209" s="1" t="s">
-        <v>364</v>
+        <v>320</v>
       </c>
       <c r="T209" t="s">
         <v>23</v>
@@ -14682,7 +14682,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="210" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>1990</v>
       </c>
@@ -14735,7 +14735,7 @@
         <v>22</v>
       </c>
       <c r="S210" s="1" t="s">
-        <v>365</v>
+        <v>386</v>
       </c>
       <c r="T210" t="s">
         <v>23</v>
@@ -14744,7 +14744,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="211" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>1990</v>
       </c>
@@ -14803,7 +14803,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="212" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>1990</v>
       </c>
@@ -14862,7 +14862,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="213" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>1990</v>
       </c>
@@ -14921,7 +14921,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="214" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>1990</v>
       </c>
@@ -14980,7 +14980,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="215" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>1990</v>
       </c>
@@ -15039,7 +15039,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="216" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>1990</v>
       </c>
@@ -15098,7 +15098,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="217" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>1990</v>
       </c>
@@ -15151,7 +15151,7 @@
         <v>22</v>
       </c>
       <c r="S217" s="1" t="s">
-        <v>366</v>
+        <v>387</v>
       </c>
       <c r="T217" t="s">
         <v>23</v>
@@ -15160,7 +15160,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="218" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>1990</v>
       </c>
@@ -15213,7 +15213,7 @@
         <v>22</v>
       </c>
       <c r="S218" s="1" t="s">
-        <v>367</v>
+        <v>321</v>
       </c>
       <c r="T218" t="s">
         <v>23</v>
@@ -15222,7 +15222,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="219" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>1990</v>
       </c>
@@ -15281,7 +15281,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="220" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>1990</v>
       </c>
@@ -15340,7 +15340,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="221" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>1990</v>
       </c>
@@ -15393,7 +15393,7 @@
         <v>22</v>
       </c>
       <c r="S221" s="1" t="s">
-        <v>368</v>
+        <v>322</v>
       </c>
       <c r="T221" t="s">
         <v>23</v>
@@ -15402,7 +15402,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="222" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>1990</v>
       </c>
@@ -15455,7 +15455,7 @@
         <v>22</v>
       </c>
       <c r="S222" s="1" t="s">
-        <v>369</v>
+        <v>323</v>
       </c>
       <c r="T222" t="s">
         <v>23</v>
@@ -15464,7 +15464,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="223" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>1990</v>
       </c>
@@ -15523,7 +15523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="224" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>1990</v>
       </c>
@@ -15582,7 +15582,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="225" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>1990</v>
       </c>
@@ -15635,7 +15635,7 @@
         <v>22</v>
       </c>
       <c r="S225" s="1" t="s">
-        <v>370</v>
+        <v>388</v>
       </c>
       <c r="T225" t="s">
         <v>23</v>
@@ -15644,7 +15644,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="226" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>1990</v>
       </c>
@@ -15697,7 +15697,7 @@
         <v>22</v>
       </c>
       <c r="S226" s="1" t="s">
-        <v>371</v>
+        <v>324</v>
       </c>
       <c r="T226" t="s">
         <v>23</v>
@@ -15706,7 +15706,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="227" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>1990</v>
       </c>
@@ -15759,7 +15759,7 @@
         <v>22</v>
       </c>
       <c r="S227" s="1" t="s">
-        <v>372</v>
+        <v>389</v>
       </c>
       <c r="T227" t="s">
         <v>23</v>
@@ -15768,7 +15768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="228" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>1990</v>
       </c>
@@ -15821,7 +15821,7 @@
         <v>22</v>
       </c>
       <c r="S228" s="1" t="s">
-        <v>373</v>
+        <v>325</v>
       </c>
       <c r="T228" t="s">
         <v>23</v>
@@ -15830,7 +15830,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="229" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>1990</v>
       </c>
@@ -15883,7 +15883,7 @@
         <v>22</v>
       </c>
       <c r="S229" s="1" t="s">
-        <v>374</v>
+        <v>326</v>
       </c>
       <c r="T229" t="s">
         <v>23</v>
@@ -15892,7 +15892,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="230" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>1990</v>
       </c>
@@ -15951,7 +15951,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="231" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>1990</v>
       </c>
@@ -16004,7 +16004,7 @@
         <v>22</v>
       </c>
       <c r="S231" s="1" t="s">
-        <v>375</v>
+        <v>327</v>
       </c>
       <c r="T231" t="s">
         <v>23</v>
@@ -16013,7 +16013,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="232" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>1990</v>
       </c>
@@ -16066,7 +16066,7 @@
         <v>22</v>
       </c>
       <c r="S232" s="1" t="s">
-        <v>376</v>
+        <v>328</v>
       </c>
       <c r="T232" t="s">
         <v>23</v>
@@ -16075,7 +16075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="233" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>1990</v>
       </c>
@@ -16128,7 +16128,7 @@
         <v>22</v>
       </c>
       <c r="S233" s="1" t="s">
-        <v>377</v>
+        <v>329</v>
       </c>
       <c r="T233" t="s">
         <v>23</v>
@@ -16137,7 +16137,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="234" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>1990</v>
       </c>
@@ -16190,7 +16190,7 @@
         <v>22</v>
       </c>
       <c r="S234" s="1" t="s">
-        <v>378</v>
+        <v>330</v>
       </c>
       <c r="T234" t="s">
         <v>23</v>
@@ -16199,7 +16199,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="235" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>1990</v>
       </c>
@@ -16258,7 +16258,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="236" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>1990</v>
       </c>
@@ -16311,7 +16311,7 @@
         <v>22</v>
       </c>
       <c r="S236" s="1" t="s">
-        <v>379</v>
+        <v>390</v>
       </c>
       <c r="T236" t="s">
         <v>23</v>
@@ -16320,7 +16320,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="237" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>1990</v>
       </c>
@@ -16379,7 +16379,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="238" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>1990</v>
       </c>
@@ -16438,7 +16438,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="239" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>1990</v>
       </c>
@@ -16497,7 +16497,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="240" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>1990</v>
       </c>
@@ -16550,7 +16550,7 @@
         <v>22</v>
       </c>
       <c r="S240" s="1" t="s">
-        <v>380</v>
+        <v>331</v>
       </c>
       <c r="T240" t="s">
         <v>23</v>
@@ -16559,7 +16559,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="241" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>1990</v>
       </c>
@@ -16618,7 +16618,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="242" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>1990</v>
       </c>
@@ -16677,7 +16677,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="243" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>1990</v>
       </c>
@@ -16736,7 +16736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="244" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>1990</v>
       </c>
@@ -16795,7 +16795,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="245" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>1990</v>
       </c>
@@ -16854,7 +16854,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="246" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>1990</v>
       </c>
@@ -16913,7 +16913,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="247" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>1990</v>
       </c>
@@ -16972,7 +16972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="248" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>1990</v>
       </c>
@@ -17031,7 +17031,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="249" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>1990</v>
       </c>
@@ -17090,7 +17090,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="250" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>1990</v>
       </c>
@@ -17149,7 +17149,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="251" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>1990</v>
       </c>
@@ -17208,7 +17208,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="252" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>1990</v>
       </c>
@@ -17267,7 +17267,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="253" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>1990</v>
       </c>
@@ -17320,7 +17320,7 @@
         <v>22</v>
       </c>
       <c r="S253" s="1" t="s">
-        <v>384</v>
+        <v>335</v>
       </c>
       <c r="T253" t="s">
         <v>23</v>
@@ -17329,7 +17329,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="254" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>1990</v>
       </c>
@@ -17382,7 +17382,7 @@
         <v>22</v>
       </c>
       <c r="S254" s="1" t="s">
-        <v>386</v>
+        <v>337</v>
       </c>
       <c r="T254" t="s">
         <v>23</v>
@@ -17391,7 +17391,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="255" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>1990</v>
       </c>
@@ -17444,7 +17444,7 @@
         <v>22</v>
       </c>
       <c r="S255" s="1" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="T255" t="s">
         <v>23</v>
@@ -17453,7 +17453,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="256" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>1990</v>
       </c>
@@ -17506,7 +17506,7 @@
         <v>22</v>
       </c>
       <c r="S256" s="1" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="T256" t="s">
         <v>23</v>
@@ -17515,7 +17515,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="257" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>1990</v>
       </c>
@@ -17547,10 +17547,10 @@
         <v>0.1</v>
       </c>
       <c r="S257" s="1" t="s">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="258" spans="1:19" x14ac:dyDescent="0.35">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="258" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>1990</v>
       </c>
@@ -17582,7 +17582,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="259" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>1990</v>
       </c>
@@ -17614,7 +17614,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="260" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>1990</v>
       </c>
@@ -17646,10 +17646,10 @@
         <v>0</v>
       </c>
       <c r="S260" s="1" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="261" spans="1:19" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="261" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>1990</v>
       </c>
@@ -17681,7 +17681,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="262" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>1990</v>
       </c>
@@ -17713,10 +17713,10 @@
         <v>0.3</v>
       </c>
       <c r="S262" s="1" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="263" spans="1:19" x14ac:dyDescent="0.35">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="263" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>1990</v>
       </c>
@@ -17748,7 +17748,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="264" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>1990</v>
       </c>
@@ -17780,7 +17780,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="265" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>1990</v>
       </c>
@@ -17812,7 +17812,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="266" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>1990</v>
       </c>
@@ -17844,7 +17844,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="267" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>1990</v>
       </c>
@@ -17876,7 +17876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>1990</v>
       </c>
@@ -17908,10 +17908,10 @@
         <v>0.5</v>
       </c>
       <c r="S268" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="269" spans="1:19" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="269" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>1990</v>
       </c>
@@ -17943,7 +17943,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="270" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>1990</v>
       </c>
@@ -17975,7 +17975,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="271" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>1990</v>
       </c>
@@ -18007,10 +18007,10 @@
         <v>0.2</v>
       </c>
       <c r="S271" s="1" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="272" spans="1:19" x14ac:dyDescent="0.35">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="272" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>1990</v>
       </c>
@@ -18042,10 +18042,10 @@
         <v>22</v>
       </c>
       <c r="S272" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="273" spans="1:19" x14ac:dyDescent="0.35">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="273" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>1990</v>
       </c>
@@ -18077,10 +18077,10 @@
         <v>22</v>
       </c>
       <c r="S273" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="274" spans="1:19" x14ac:dyDescent="0.35">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="274" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>1990</v>
       </c>
@@ -18112,10 +18112,10 @@
         <v>22</v>
       </c>
       <c r="S274" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="275" spans="1:19" x14ac:dyDescent="0.35">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="275" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>1990</v>
       </c>
@@ -18147,10 +18147,10 @@
         <v>22</v>
       </c>
       <c r="S275" s="1" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="276" spans="1:19" x14ac:dyDescent="0.35">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="276" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>1990</v>
       </c>
@@ -18182,7 +18182,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="277" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>1990</v>
       </c>
@@ -18214,7 +18214,7 @@
         <v>1.7</v>
       </c>
     </row>
-    <row r="278" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>1990</v>
       </c>
@@ -18246,7 +18246,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="279" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>1990</v>
       </c>
@@ -18278,10 +18278,10 @@
         <v>22</v>
       </c>
       <c r="S279" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="280" spans="1:19" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="280" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>1990</v>
       </c>
@@ -18313,10 +18313,10 @@
         <v>22</v>
       </c>
       <c r="S280" s="1" t="s">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="281" spans="1:19" x14ac:dyDescent="0.35">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="281" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>1990</v>
       </c>
@@ -18348,7 +18348,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="282" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>1990</v>
       </c>
@@ -18380,7 +18380,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="283" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>1990</v>
       </c>
@@ -18412,7 +18412,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="284" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>1990</v>
       </c>
@@ -18444,7 +18444,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="285" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>1990</v>
       </c>
@@ -18476,7 +18476,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="286" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>1990</v>
       </c>
@@ -18508,10 +18508,10 @@
         <v>-0.1</v>
       </c>
       <c r="S286" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="287" spans="1:19" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="287" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>1990</v>
       </c>
@@ -18546,7 +18546,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="288" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>1990</v>
       </c>
@@ -18581,7 +18581,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="289" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>1990</v>
       </c>
@@ -18616,7 +18616,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="290" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>1990</v>
       </c>
@@ -18648,10 +18648,10 @@
         <v>22</v>
       </c>
       <c r="S290" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="291" spans="1:19" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="291" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>1990</v>
       </c>
@@ -18686,7 +18686,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="292" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>1990</v>
       </c>
@@ -18721,7 +18721,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="293" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>1990</v>
       </c>
@@ -18756,7 +18756,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="294" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>1990</v>
       </c>
@@ -18788,10 +18788,10 @@
         <v>22</v>
       </c>
       <c r="S294" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="295" spans="1:19" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="295" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>1990</v>
       </c>
@@ -18823,10 +18823,10 @@
         <v>22</v>
       </c>
       <c r="S295" s="1" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="296" spans="1:19" x14ac:dyDescent="0.35">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="296" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>1990</v>
       </c>
@@ -18858,7 +18858,7 @@
         <v>22</v>
       </c>
       <c r="S296" s="1" t="s">
-        <v>392</v>
+        <v>341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>